<commit_message>
First round of experimental data generated
</commit_message>
<xml_diff>
--- a/Experiments/ExperimentLog.xlsx
+++ b/Experiments/ExperimentLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oeide/Documents/GitHub/space-exploration/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDC6BAD-EF96-9A45-A621-FE0A7CA1A007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A03CB93-7EA3-A940-BF3A-EB8EAC0BFE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13420" yWindow="-33340" windowWidth="28240" windowHeight="19920" xr2:uid="{2C80AC6F-9F2E-6B48-92A8-47CFE9D5C5D5}"/>
+    <workbookView xWindow="2660" yWindow="780" windowWidth="28240" windowHeight="19920" xr2:uid="{2C80AC6F-9F2E-6B48-92A8-47CFE9D5C5D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Experiment</t>
   </si>
@@ -65,6 +65,78 @@
   </si>
   <si>
     <t>1, 2, 4, 5</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 5, 6</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 7, 8, 9</t>
+  </si>
+  <si>
+    <t>Off1</t>
+  </si>
+  <si>
+    <t>Off2</t>
+  </si>
+  <si>
+    <t>Off3</t>
+  </si>
+  <si>
+    <t>Off4</t>
+  </si>
+  <si>
+    <t>Off5</t>
+  </si>
+  <si>
+    <t>Off6</t>
+  </si>
+  <si>
+    <t>Bygd1</t>
+  </si>
+  <si>
+    <t>Bygd2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Bygd3</t>
+  </si>
+  <si>
+    <t>Bygd4</t>
+  </si>
+  <si>
+    <t>2, 6</t>
+  </si>
+  <si>
+    <t>Bygd5</t>
+  </si>
+  <si>
+    <t>2, 3, 6</t>
+  </si>
+  <si>
+    <t>Bygd6</t>
+  </si>
+  <si>
+    <t>2, 3, 6, 8</t>
+  </si>
+  <si>
+    <t>Bygd7</t>
+  </si>
+  <si>
+    <t>Fjell1</t>
+  </si>
+  <si>
+    <t>Fjell2</t>
+  </si>
+  <si>
+    <t>Fjell3</t>
+  </si>
+  <si>
+    <t>Fjell4</t>
   </si>
 </sst>
 </file>
@@ -439,7 +511,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,8 +544,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -496,8 +568,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
         <v>45</v>
@@ -520,8 +592,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4">
         <v>90</v>
@@ -544,8 +616,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>16</v>
       </c>
       <c r="B5">
         <v>135</v>
@@ -553,41 +625,81 @@
       <c r="C5">
         <v>11.3</v>
       </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.555555555555557</v>
       </c>
       <c r="G5">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>180</v>
+      </c>
       <c r="C6">
         <v>11.3</v>
       </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="G6">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>225</v>
+      </c>
       <c r="C7">
         <v>11.3</v>
       </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G7">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
       <c r="C8">
-        <v>11.3</v>
+        <v>8</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8">
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
@@ -598,8 +710,17 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
       <c r="C9">
-        <v>11.3</v>
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
@@ -610,54 +731,138 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>90</v>
+      </c>
       <c r="C10">
-        <v>11.3</v>
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11.111111111111111</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>135</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.222222222222221</v>
       </c>
       <c r="G11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>180</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="G12">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>225</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44.444444444444443</v>
       </c>
       <c r="G13">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>270</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44.444444444444443</v>
       </c>
       <c r="G14">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>90</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -667,6 +872,18 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>135</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -675,7 +892,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>180</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -684,7 +913,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>225</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -693,7 +934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -702,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -711,7 +952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -720,7 +961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -729,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -738,7 +979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -747,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -756,7 +997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -765,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -774,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -783,7 +1024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -792,7 +1033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Wrong data corrected, experiments re-ran
One place had wrong coordinates
</commit_message>
<xml_diff>
--- a/Experiments/ExperimentLog.xlsx
+++ b/Experiments/ExperimentLog.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oeide/Documents/GitHub/space-exploration/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A03CB93-7EA3-A940-BF3A-EB8EAC0BFE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08AB5CE-3C0F-904A-8162-E860D6566A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="780" windowWidth="28240" windowHeight="19920" xr2:uid="{2C80AC6F-9F2E-6B48-92A8-47CFE9D5C5D5}"/>
+    <workbookView xWindow="11840" yWindow="8520" windowWidth="22360" windowHeight="13580" xr2:uid="{2C80AC6F-9F2E-6B48-92A8-47CFE9D5C5D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,23 +35,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Experiment</t>
   </si>
   <si>
-    <t>span</t>
-  </si>
-  <si>
-    <t>distMiil</t>
-  </si>
-  <si>
     <t>Overlap</t>
   </si>
   <si>
-    <t>Success rate</t>
-  </si>
-  <si>
     <t>Σ</t>
   </si>
   <si>
@@ -61,9 +52,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>1, 4</t>
-  </si>
-  <si>
     <t>1, 2, 4, 5</t>
   </si>
   <si>
@@ -109,24 +97,12 @@
     <t>Bygd4</t>
   </si>
   <si>
-    <t>2, 6</t>
-  </si>
-  <si>
     <t>Bygd5</t>
   </si>
   <si>
-    <t>2, 3, 6</t>
-  </si>
-  <si>
     <t>Bygd6</t>
   </si>
   <si>
-    <t>2, 3, 6, 8</t>
-  </si>
-  <si>
-    <t>Bygd7</t>
-  </si>
-  <si>
     <t>Fjell1</t>
   </si>
   <si>
@@ -137,6 +113,57 @@
   </si>
   <si>
     <t>Fjell4</t>
+  </si>
+  <si>
+    <t>Match place</t>
+  </si>
+  <si>
+    <t># match</t>
+  </si>
+  <si>
+    <t>Match rate</t>
+  </si>
+  <si>
+    <t>Overlap rate</t>
+  </si>
+  <si>
+    <t>1, 4, 5</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5, 8</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Off7</t>
+  </si>
+  <si>
+    <t>2, 4, 5</t>
+  </si>
+  <si>
+    <t>2, 4, 5, 6</t>
+  </si>
+  <si>
+    <t>2, 4, 5, 6, 8</t>
+  </si>
+  <si>
+    <t>Fjell5</t>
+  </si>
+  <si>
+    <t>Span</t>
+  </si>
+  <si>
+    <t>Miil</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -508,68 +535,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A452142E-4A9B-7E49-9DFB-7E62EBFA6EAC}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>11.3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <f>E2/G2*100</f>
+        <f>E2/J2*100</f>
         <v>11.111111111111111</v>
       </c>
-      <c r="G2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <f>H2/J2*100</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>45</v>
@@ -578,22 +626,29 @@
         <v>11.3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F30" si="0">E3/G3*100</f>
-        <v>22.222222222222221</v>
-      </c>
-      <c r="G3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F3:F18" si="0">E3/J3*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I19" si="1">H3/J3*100</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>90</v>
@@ -602,7 +657,7 @@
         <v>11.3</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -611,13 +666,23 @@
         <f t="shared" si="0"/>
         <v>44.444444444444443</v>
       </c>
-      <c r="G4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>135</v>
@@ -626,7 +691,7 @@
         <v>11.3</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -635,13 +700,23 @@
         <f t="shared" si="0"/>
         <v>55.555555555555557</v>
       </c>
-      <c r="G5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>180</v>
@@ -650,7 +725,7 @@
         <v>11.3</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -659,13 +734,23 @@
         <f t="shared" si="0"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="G6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>225</v>
@@ -674,7 +759,7 @@
         <v>11.3</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -683,42 +768,65 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B8">
+        <v>270</v>
+      </c>
+      <c r="C8">
+        <v>11.3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" ref="F8" si="2">E8/J8*100</f>
+        <v>100</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
       <c r="B9">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
+      <c r="D9" s="5"/>
       <c r="E9">
         <v>0</v>
       </c>
@@ -726,94 +834,122 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
+      <c r="D10" t="s">
+        <v>32</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="G10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22.222222222222221</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>24</v>
+      <c r="D11" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>22.222222222222221</v>
-      </c>
-      <c r="G11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="C12">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>33.333333333333329</v>
-      </c>
-      <c r="G12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>44.444444444444443</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="C13">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -822,40 +958,57 @@
         <f t="shared" si="0"/>
         <v>44.444444444444443</v>
       </c>
-      <c r="G13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>44.444444444444443</v>
-      </c>
-      <c r="G14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -867,180 +1020,173 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B16">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="C16">
         <v>6</v>
       </c>
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B17">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
+      <c r="D17" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B18">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
+      <c r="D18" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>225</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
       <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>9</v>
-      </c>
+        <f t="shared" ref="F19" si="3">E19/J19*100</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>